<commit_message>
Included screenshots for html report and excel data set input
</commit_message>
<xml_diff>
--- a/Aldo-Test-Data-set.xlsx
+++ b/Aldo-Test-Data-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hari4\python-webui-filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAA38E7-2215-428F-A1A5-F625E9F07D6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B14D18-825C-4BB8-B3E4-4E3C8215693D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EDF5FB46-B36E-40B2-AB95-F94766D28BEB}"/>
   </bookViews>
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,10 +176,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -198,16 +211,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,7 +556,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C1" sqref="C1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,197 +575,200 @@
     <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="b">
+      <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M2">
+      <c r="L2" s="2"/>
+      <c r="M2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="b">
+      <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M3">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="b">
+      <c r="C4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="4">
         <v>7</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="b">
+      <c r="C5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M5">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2">
         <v>2</v>
       </c>
     </row>
@@ -752,21 +785,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F65BFE220852654A94B0E24FAB8D414F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bdacad30f1d04398aad8d480b298e327">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7a2423e-e457-463e-bb09-ea35f27c79d5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d7967f50696128c4f60bd15feea58994" ns3:_="">
     <xsd:import namespace="b7a2423e-e457-463e-bb09-ea35f27c79d5"/>
@@ -936,24 +954,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26CAAAA5-B919-4882-8B55-7BA28EC43444}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04331AB7-27E2-427E-B974-CFD943DB3B3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FF27198-C35E-49FE-AC2C-C7F5925F492B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -969,4 +985,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04331AB7-27E2-427E-B974-CFD943DB3B3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26CAAAA5-B919-4882-8B55-7BA28EC43444}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>